<commit_message>
Semi-completed thesis document, addition of Scheduled Shared Experience
</commit_message>
<xml_diff>
--- a/Proposed Architecture/results.xlsx
+++ b/Proposed Architecture/results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12940"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="54">
   <si>
     <t>DAL</t>
   </si>
@@ -137,9 +137,6 @@
     <t>Same</t>
   </si>
   <si>
-    <t>2\9</t>
-  </si>
-  <si>
     <t>23\125</t>
   </si>
   <si>
@@ -162,6 +159,33 @@
   </si>
   <si>
     <t>13\95</t>
+  </si>
+  <si>
+    <t>0\10</t>
+  </si>
+  <si>
+    <t>9\95</t>
+  </si>
+  <si>
+    <t>1000 with 50 episodes each</t>
+  </si>
+  <si>
+    <t>1\10</t>
+  </si>
+  <si>
+    <t>8\125</t>
+  </si>
+  <si>
+    <t>Need to try without pooling and greater number of epochs</t>
+  </si>
+  <si>
+    <t>DAL (no pooling)</t>
+  </si>
+  <si>
+    <t>DQN-DQN-SCH-EXP</t>
+  </si>
+  <si>
+    <t>DDQN-SCH-EXP</t>
   </si>
 </sst>
 </file>
@@ -535,11 +559,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y8"/>
+  <dimension ref="A1:Y12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -553,7 +577,7 @@
     <col min="7" max="7" width="7.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.6328125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6.81640625" style="1" bestFit="1" customWidth="1"/>
@@ -638,167 +662,168 @@
       </c>
       <c r="Y1" s="5"/>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>42869</v>
+      </c>
+      <c r="D2" s="1">
+        <v>800</v>
+      </c>
+      <c r="E2" s="1">
+        <v>200</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="1">
+        <v>100</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T2" s="1">
+        <v>10</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
-    <row r="3" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C4" s="3">
         <v>42867</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D4" s="1">
         <v>8000</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E4" s="1">
         <v>2000</v>
       </c>
-      <c r="F3" s="1">
-        <v>10000</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="F4" s="1">
+        <v>10000</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I4" s="1">
         <v>100</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="1">
-        <v>10000</v>
-      </c>
-      <c r="L3" s="1">
-        <v>10000</v>
-      </c>
-      <c r="M3" s="1" t="s">
+      <c r="K4" s="1">
+        <v>10000</v>
+      </c>
+      <c r="L4" s="1">
+        <v>10000</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="1">
+      <c r="N4" s="1">
         <v>0.01</v>
       </c>
-      <c r="O3" s="1">
+      <c r="O4" s="1">
         <v>0.9</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="T3" s="4">
+      <c r="T4" s="4">
         <v>10</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="U4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="W3" s="1">
+      <c r="W4" s="1">
         <v>5800</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="X4" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:25" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3">
-        <v>42868</v>
-      </c>
-      <c r="D5" s="1">
-        <v>10000</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="1">
-        <v>100</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K5" s="1">
-        <v>10000</v>
-      </c>
-      <c r="L5" s="1">
-        <v>10000</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N5" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="O5" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="P5" s="1">
-        <v>1000</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S5" s="1">
-        <v>500</v>
-      </c>
-      <c r="T5" s="1">
-        <v>10</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="W5" s="1">
-        <v>4400</v>
-      </c>
-      <c r="X5" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
@@ -807,7 +832,7 @@
         <v>42868</v>
       </c>
       <c r="D6" s="1">
-        <v>1000</v>
+        <v>10000</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
@@ -828,7 +853,7 @@
         <v>27</v>
       </c>
       <c r="K6" s="1">
-        <v>1500</v>
+        <v>10000</v>
       </c>
       <c r="L6" s="1">
         <v>10000</v>
@@ -837,7 +862,7 @@
         <v>28</v>
       </c>
       <c r="N6" s="1">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="O6" s="1">
         <v>0.9</v>
@@ -858,24 +883,24 @@
         <v>10</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="W6" s="1">
-        <v>8500</v>
+        <v>4400</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" ht="29" x14ac:dyDescent="0.35">
       <c r="B7" s="1">
         <v>1</v>
       </c>
       <c r="C7" s="3">
-        <v>42868</v>
+        <v>42869</v>
       </c>
       <c r="D7" s="1">
         <v>8000</v>
@@ -908,7 +933,7 @@
         <v>28</v>
       </c>
       <c r="N7" s="1">
-        <v>1E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="O7" s="1">
         <v>0.9</v>
@@ -929,87 +954,242 @@
         <v>10</v>
       </c>
       <c r="U7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="W7" s="1">
+        <v>3600</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>42868</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="1">
+        <v>100</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1500</v>
+      </c>
+      <c r="L9" s="1">
+        <v>10000</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="P9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S9" s="1">
+        <v>500</v>
+      </c>
+      <c r="T9" s="1">
+        <v>10</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W9" s="1">
+        <v>8500</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B10" s="1">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3">
+        <v>42868</v>
+      </c>
+      <c r="D10" s="1">
+        <v>8000</v>
+      </c>
+      <c r="E10" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I10" s="1">
+        <v>100</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="1">
+        <v>10000</v>
+      </c>
+      <c r="L10" s="1">
+        <v>10000</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="P10" s="1">
+        <v>1000</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S10" s="1">
+        <v>500</v>
+      </c>
+      <c r="T10" s="1">
+        <v>10</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="W10" s="1">
+        <v>4500</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B11" s="1">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3">
+        <v>42868</v>
+      </c>
+      <c r="D11" s="1">
+        <v>8000</v>
+      </c>
+      <c r="E11" s="1">
+        <v>2000</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="1">
+        <v>100</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="1">
+        <v>10000</v>
+      </c>
+      <c r="L11" s="1">
+        <v>10000</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="P11" s="1">
+        <v>1000</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="R11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S11" s="1">
+        <v>500</v>
+      </c>
+      <c r="T11" s="1">
+        <v>10</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="V11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="V7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="W7" s="1">
-        <v>4500</v>
-      </c>
-      <c r="X7" s="1" t="s">
-        <v>41</v>
+      <c r="W11" s="1">
+        <v>8200</v>
+      </c>
+      <c r="X11" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B8" s="1">
-        <v>2</v>
-      </c>
-      <c r="C8" s="3">
-        <v>42868</v>
-      </c>
-      <c r="D8" s="1">
-        <v>8000</v>
-      </c>
-      <c r="E8" s="1">
-        <v>2000</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="1">
-        <v>100</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K8" s="1">
-        <v>10000</v>
-      </c>
-      <c r="L8" s="1">
-        <v>10000</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N8" s="1">
-        <v>1E-3</v>
-      </c>
-      <c r="O8" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="P8" s="1">
-        <v>1000</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="S8" s="1">
-        <v>500</v>
-      </c>
-      <c r="T8" s="1">
-        <v>10</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="W8" s="1">
-        <v>8200</v>
-      </c>
-      <c r="X8" s="1" t="s">
-        <v>41</v>
+    <row r="12" spans="1:25" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Semi-finished thesis document, updated DRQN implementation
</commit_message>
<xml_diff>
--- a/Proposed Architecture/results.xlsx
+++ b/Proposed Architecture/results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="74">
   <si>
     <t>DAL</t>
   </si>
@@ -237,13 +237,22 @@
   </si>
   <si>
     <t>7\95</t>
+  </si>
+  <si>
+    <t>DRQN-AL</t>
+  </si>
+  <si>
+    <t>19\95</t>
+  </si>
+  <si>
+    <t>8 episodes, 4 length</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,6 +262,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -281,20 +297,20 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment textRotation="255" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -610,1451 +626,1599 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y20"/>
+  <dimension ref="A1:Y23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V4" sqref="V4"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W26" sqref="W26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="3.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="9.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="6.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="3.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.1796875" style="3" customWidth="1"/>
+    <col min="18" max="18" width="7.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="2" customFormat="1" ht="137.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="O1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="T1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="U1" s="5" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="W1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="X1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="Y1" s="5"/>
+      <c r="Y1" s="1"/>
     </row>
     <row r="2" spans="1:25" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>42869</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="3">
         <v>800</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="3">
         <v>200</v>
       </c>
-      <c r="F2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="3">
+        <v>1000</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="3">
         <v>100</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="1">
+      <c r="N2" s="3">
         <v>0.01</v>
       </c>
-      <c r="O2" s="1">
+      <c r="O2" s="3">
         <v>0.9</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="R2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="S2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="T2" s="1">
+      <c r="T2" s="3">
         <v>10</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="U2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="V2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="W2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="X2" s="1" t="s">
+      <c r="W2" s="3">
+        <v>1000</v>
+      </c>
+      <c r="X2" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="87" x14ac:dyDescent="0.35">
-      <c r="B3" s="1">
+      <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>42869</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="3">
         <v>800</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="3">
         <v>200</v>
       </c>
-      <c r="F3" s="1">
-        <v>1000</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="F3" s="3">
+        <v>1000</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="3">
         <v>100</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="1">
+      <c r="N3" s="3">
         <v>0.01</v>
       </c>
-      <c r="O3" s="1">
+      <c r="O3" s="3">
         <v>0.9</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="R3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="S3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="T3" s="1">
+      <c r="T3" s="3">
         <v>10</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="U3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="V3" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="W3" s="1">
-        <v>1000</v>
-      </c>
-      <c r="X3" s="1" t="s">
+      <c r="W3" s="3">
+        <v>1000</v>
+      </c>
+      <c r="X3" s="3" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="4">
         <v>42867</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="3">
         <v>8000</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="3">
         <v>2000</v>
       </c>
-      <c r="F4" s="1">
-        <v>10000</v>
-      </c>
-      <c r="G4" s="1" t="s">
+      <c r="F4" s="3">
+        <v>10000</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="3">
         <v>100</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="1">
-        <v>10000</v>
-      </c>
-      <c r="L4" s="1">
-        <v>10000</v>
-      </c>
-      <c r="M4" s="1" t="s">
+      <c r="K4" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L4" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="1">
+      <c r="N4" s="3">
         <v>0.01</v>
       </c>
-      <c r="O4" s="1">
+      <c r="O4" s="3">
         <v>0.9</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="P4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="Q4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="R4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="S4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="T4" s="4">
+      <c r="T4" s="5">
         <v>10</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="U4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="V4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W4" s="1">
+      <c r="W4" s="3">
         <v>5800</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="X4" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B5" s="1">
+      <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="4">
         <v>42871</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="3">
         <v>800</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="3">
         <v>200</v>
       </c>
-      <c r="F5" s="1">
-        <v>1000</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="F5" s="3">
+        <v>1000</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="3">
         <v>100</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K5" s="1">
-        <v>10000</v>
-      </c>
-      <c r="L5" s="1">
-        <v>10000</v>
-      </c>
-      <c r="M5" s="1" t="s">
+      <c r="K5" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L5" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="1">
+      <c r="N5" s="3">
         <v>0.01</v>
       </c>
-      <c r="O5" s="1">
+      <c r="O5" s="3">
         <v>0.9</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="R5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="S5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="T5" s="4">
+      <c r="T5" s="5">
         <v>10</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="U5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="V5" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="W5" s="1">
+      <c r="W5" s="3">
         <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="3">
         <v>1</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="4">
         <v>42871</v>
       </c>
-      <c r="D6" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1" t="s">
+      <c r="D6" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="3">
         <v>100</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K6" s="1">
-        <v>10000</v>
-      </c>
-      <c r="L6" s="1">
-        <v>10000</v>
-      </c>
-      <c r="M6" s="1" t="s">
+      <c r="K6" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L6" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N6" s="1">
+      <c r="N6" s="3">
         <v>0.1</v>
       </c>
-      <c r="O6" s="1">
+      <c r="O6" s="3">
         <v>0.9</v>
       </c>
-      <c r="P6" s="1">
-        <v>1000</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>0</v>
-      </c>
-      <c r="R6" s="1" t="s">
+      <c r="P6" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0</v>
+      </c>
+      <c r="R6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="S6" s="1">
+      <c r="S6" s="3">
         <v>500</v>
       </c>
-      <c r="T6" s="1">
+      <c r="T6" s="3">
         <v>10</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="U6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="V6" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="W6" s="1">
+      <c r="W6" s="3">
         <v>900</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B7" s="1">
+      <c r="B7" s="3">
         <v>1</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="4">
         <v>42871</v>
       </c>
-      <c r="D7" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1" t="s">
+      <c r="D7" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="3">
         <v>100</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K7" s="1">
-        <v>10000</v>
-      </c>
-      <c r="L7" s="1">
-        <v>10000</v>
-      </c>
-      <c r="M7" s="1" t="s">
+      <c r="K7" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L7" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N7" s="1">
+      <c r="N7" s="3">
         <v>0.01</v>
       </c>
-      <c r="O7" s="1">
+      <c r="O7" s="3">
         <v>0.9</v>
       </c>
-      <c r="P7" s="1">
-        <v>1000</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>0</v>
-      </c>
-      <c r="R7" s="1" t="s">
+      <c r="P7" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>0</v>
+      </c>
+      <c r="R7" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="S7" s="1">
+      <c r="S7" s="3">
         <v>500</v>
       </c>
-      <c r="T7" s="1">
+      <c r="T7" s="3">
         <v>10</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="U7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="V7" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="W7" s="1">
+      <c r="W7" s="3">
         <v>3000</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="B8" s="1">
+      <c r="B8" s="3">
         <v>1</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="4">
         <v>42871</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="3">
         <v>8000</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="3">
         <v>2000</v>
       </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1" t="s">
+      <c r="F8" s="3">
+        <v>0</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="3">
         <v>100</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K8" s="1">
-        <v>10000</v>
-      </c>
-      <c r="L8" s="1">
-        <v>10000</v>
-      </c>
-      <c r="M8" s="1" t="s">
+      <c r="K8" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L8" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N8" s="1">
+      <c r="N8" s="3">
         <v>0.01</v>
       </c>
-      <c r="O8" s="1">
+      <c r="O8" s="3">
         <v>0.9</v>
       </c>
-      <c r="P8" s="1">
-        <v>1000</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>0</v>
-      </c>
-      <c r="R8" s="1" t="s">
+      <c r="P8" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>0</v>
+      </c>
+      <c r="R8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="S8" s="1">
+      <c r="S8" s="3">
         <v>500</v>
       </c>
-      <c r="T8" s="1">
+      <c r="T8" s="3">
         <v>10</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="U8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="V8" s="1" t="s">
+      <c r="V8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="W8" s="1">
+      <c r="W8" s="3">
         <v>1200</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="3">
         <v>1</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="4">
         <v>42868</v>
       </c>
-      <c r="D9" s="1">
-        <v>10000</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1" t="s">
+      <c r="D9" s="3">
+        <v>10000</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="3">
         <v>100</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="1">
-        <v>10000</v>
-      </c>
-      <c r="L9" s="1">
-        <v>10000</v>
-      </c>
-      <c r="M9" s="1" t="s">
+      <c r="K9" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L9" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N9" s="1">
+      <c r="N9" s="3">
         <v>1E-3</v>
       </c>
-      <c r="O9" s="1">
+      <c r="O9" s="3">
         <v>0.9</v>
       </c>
-      <c r="P9" s="1">
-        <v>1000</v>
-      </c>
-      <c r="Q9" s="1">
+      <c r="P9" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q9" s="3">
         <v>0.1</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="R9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="S9" s="1">
+      <c r="S9" s="3">
         <v>500</v>
       </c>
-      <c r="T9" s="1">
+      <c r="T9" s="3">
         <v>10</v>
       </c>
-      <c r="U9" s="1" t="s">
+      <c r="U9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="V9" s="1" t="s">
+      <c r="V9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="W9" s="1">
+      <c r="W9" s="3">
         <v>4400</v>
       </c>
-      <c r="X9" s="1" t="s">
+      <c r="X9" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="29" x14ac:dyDescent="0.35">
-      <c r="B10" s="1">
+      <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="4">
         <v>42869</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="3">
         <v>8000</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="3">
         <v>2000</v>
       </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1" t="s">
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="3">
         <v>100</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="1">
-        <v>10000</v>
-      </c>
-      <c r="L10" s="1">
-        <v>10000</v>
-      </c>
-      <c r="M10" s="1" t="s">
+      <c r="K10" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L10" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N10" s="1">
+      <c r="N10" s="3">
         <v>1E-3</v>
       </c>
-      <c r="O10" s="1">
+      <c r="O10" s="3">
         <v>0.9</v>
       </c>
-      <c r="P10" s="1">
-        <v>1000</v>
-      </c>
-      <c r="Q10" s="1">
+      <c r="P10" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q10" s="3">
         <v>0.1</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="R10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="S10" s="1">
+      <c r="S10" s="3">
         <v>500</v>
       </c>
-      <c r="T10" s="1">
+      <c r="T10" s="3">
         <v>10</v>
       </c>
-      <c r="U10" s="1" t="s">
+      <c r="U10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="V10" s="1" t="s">
+      <c r="V10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="W10" s="1">
+      <c r="W10" s="3">
         <v>3600</v>
       </c>
-      <c r="X10" s="1" t="s">
+      <c r="X10" s="3" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="58" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="3">
         <v>1</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="4">
         <v>42871</v>
       </c>
-      <c r="D11" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1" t="s">
+      <c r="D11" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="3">
         <v>100</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="1">
-        <v>10000</v>
-      </c>
-      <c r="L11" s="1">
-        <v>10000</v>
-      </c>
-      <c r="M11" s="1" t="s">
+      <c r="K11" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L11" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N11" s="1">
+      <c r="N11" s="3">
         <v>1E-3</v>
       </c>
-      <c r="O11" s="1">
+      <c r="O11" s="3">
         <v>0.9</v>
       </c>
-      <c r="P11" s="1">
-        <v>1000</v>
-      </c>
-      <c r="Q11" s="1" t="s">
+      <c r="P11" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q11" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="R11" s="1" t="s">
+      <c r="R11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="S11" s="1">
+      <c r="S11" s="3">
         <v>500</v>
       </c>
-      <c r="T11" s="1">
+      <c r="T11" s="3">
         <v>10</v>
       </c>
-      <c r="U11" s="1" t="s">
+      <c r="U11" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="V11" s="1" t="s">
+      <c r="V11" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="W11" s="1">
+      <c r="W11" s="3">
         <v>3500</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="58" x14ac:dyDescent="0.35">
-      <c r="B12" s="1">
+      <c r="B12" s="3">
         <v>2</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="4">
         <v>42872</v>
       </c>
-      <c r="D12" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1" t="s">
+      <c r="D12" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="3">
         <v>100</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K12" s="1">
-        <v>10000</v>
-      </c>
-      <c r="L12" s="1">
-        <v>10000</v>
-      </c>
-      <c r="M12" s="1" t="s">
+      <c r="K12" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L12" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N12" s="1">
+      <c r="N12" s="3">
         <v>1E-3</v>
       </c>
-      <c r="O12" s="1">
+      <c r="O12" s="3">
         <v>0.9</v>
       </c>
-      <c r="P12" s="1">
-        <v>1000</v>
-      </c>
-      <c r="Q12" s="1" t="s">
+      <c r="P12" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="R12" s="1" t="s">
+      <c r="R12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="S12" s="1">
+      <c r="S12" s="3">
         <v>500</v>
       </c>
-      <c r="T12" s="1">
+      <c r="T12" s="3">
         <v>10</v>
       </c>
-      <c r="U12" s="1" t="s">
+      <c r="U12" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="V12" s="1" t="s">
+      <c r="V12" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="W12" s="1">
+      <c r="W12" s="3">
         <v>9900</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="58" x14ac:dyDescent="0.35">
-      <c r="B13" s="1">
+      <c r="B13" s="3">
         <v>1</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="4">
         <v>42873</v>
       </c>
-      <c r="D13" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1" t="s">
+      <c r="D13" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="3">
         <v>100</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K13" s="1">
-        <v>10000</v>
-      </c>
-      <c r="L13" s="1">
-        <v>10000</v>
-      </c>
-      <c r="M13" s="1" t="s">
+      <c r="K13" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L13" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N13" s="1">
+      <c r="N13" s="3">
         <v>1E-3</v>
       </c>
-      <c r="O13" s="1">
+      <c r="O13" s="3">
         <v>0.9</v>
       </c>
-      <c r="P13" s="1">
-        <v>1000</v>
-      </c>
-      <c r="Q13" s="1" t="s">
+      <c r="P13" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q13" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="R13" s="1" t="s">
+      <c r="R13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="S13" s="1">
+      <c r="S13" s="3">
         <v>500</v>
       </c>
-      <c r="T13" s="1">
+      <c r="T13" s="3">
         <v>10</v>
       </c>
-      <c r="U13" s="1" t="s">
+      <c r="U13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="V13" s="1" t="s">
+      <c r="V13" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="W13" s="1">
+      <c r="W13" s="3">
         <v>3700</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="3">
         <v>1</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="4">
         <v>42868</v>
       </c>
-      <c r="D14" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0</v>
-      </c>
-      <c r="F14" s="1">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1" t="s">
+      <c r="D14" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="H14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14" s="3">
         <v>100</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="J14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="3">
         <v>1500</v>
       </c>
-      <c r="L14" s="1">
-        <v>10000</v>
-      </c>
-      <c r="M14" s="1" t="s">
+      <c r="L14" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N14" s="1">
+      <c r="N14" s="3">
         <v>1E-4</v>
       </c>
-      <c r="O14" s="1">
+      <c r="O14" s="3">
         <v>0.9</v>
       </c>
-      <c r="P14" s="1">
-        <v>1000</v>
-      </c>
-      <c r="Q14" s="1">
+      <c r="P14" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q14" s="3">
         <v>0.1</v>
       </c>
-      <c r="R14" s="1" t="s">
+      <c r="R14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="S14" s="1">
+      <c r="S14" s="3">
         <v>500</v>
       </c>
-      <c r="T14" s="1">
+      <c r="T14" s="3">
         <v>10</v>
       </c>
-      <c r="U14" s="1" t="s">
+      <c r="U14" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="V14" s="1" t="s">
+      <c r="V14" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="W14" s="1">
+      <c r="W14" s="3">
         <v>8500</v>
       </c>
-      <c r="X14" s="1" t="s">
+      <c r="X14" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B15" s="1">
+      <c r="B15" s="3">
         <v>1</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="4">
         <v>42868</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="3">
         <v>8000</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="3">
         <v>2000</v>
       </c>
-      <c r="F15" s="1">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1" t="s">
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="3">
         <v>100</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="J15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K15" s="1">
-        <v>10000</v>
-      </c>
-      <c r="L15" s="1">
-        <v>10000</v>
-      </c>
-      <c r="M15" s="1" t="s">
+      <c r="K15" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L15" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N15" s="1">
+      <c r="N15" s="3">
         <v>1E-4</v>
       </c>
-      <c r="O15" s="1">
+      <c r="O15" s="3">
         <v>0.9</v>
       </c>
-      <c r="P15" s="1">
-        <v>1000</v>
-      </c>
-      <c r="Q15" s="1">
+      <c r="P15" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q15" s="3">
         <v>0.1</v>
       </c>
-      <c r="R15" s="1" t="s">
+      <c r="R15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="S15" s="1">
+      <c r="S15" s="3">
         <v>500</v>
       </c>
-      <c r="T15" s="1">
+      <c r="T15" s="3">
         <v>10</v>
       </c>
-      <c r="U15" s="1" t="s">
+      <c r="U15" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="V15" s="1" t="s">
+      <c r="V15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="W15" s="1">
+      <c r="W15" s="3">
         <v>4500</v>
       </c>
-      <c r="X15" s="1" t="s">
+      <c r="X15" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B16" s="1">
+      <c r="B16" s="3">
         <v>2</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="4">
         <v>42868</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="3">
         <v>8000</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="3">
         <v>2000</v>
       </c>
-      <c r="F16" s="1">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1" t="s">
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16" s="3">
         <v>100</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="J16" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K16" s="1">
-        <v>10000</v>
-      </c>
-      <c r="L16" s="1">
-        <v>10000</v>
-      </c>
-      <c r="M16" s="1" t="s">
+      <c r="K16" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L16" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N16" s="1">
+      <c r="N16" s="3">
         <v>1E-3</v>
       </c>
-      <c r="O16" s="1">
+      <c r="O16" s="3">
         <v>0.9</v>
       </c>
-      <c r="P16" s="1">
-        <v>1000</v>
-      </c>
-      <c r="Q16" s="1">
+      <c r="P16" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q16" s="3">
         <v>0.1</v>
       </c>
-      <c r="R16" s="1" t="s">
+      <c r="R16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="S16" s="1">
+      <c r="S16" s="3">
         <v>500</v>
       </c>
-      <c r="T16" s="1">
+      <c r="T16" s="3">
         <v>10</v>
       </c>
-      <c r="U16" s="1" t="s">
+      <c r="U16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="V16" s="1" t="s">
+      <c r="V16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="W16" s="1">
+      <c r="W16" s="3">
         <v>8200</v>
       </c>
-      <c r="X16" s="1" t="s">
+      <c r="X16" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:24" ht="58" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17" s="3">
         <v>1</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="4">
         <v>42871</v>
       </c>
-      <c r="D17" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1" t="s">
+      <c r="D17" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17" s="3">
         <v>100</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="J17" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K17" s="1">
-        <v>10000</v>
-      </c>
-      <c r="L17" s="1">
-        <v>10000</v>
-      </c>
-      <c r="M17" s="1" t="s">
+      <c r="K17" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L17" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M17" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N17" s="1">
+      <c r="N17" s="3">
         <v>1E-3</v>
       </c>
-      <c r="O17" s="1">
+      <c r="O17" s="3">
         <v>0.9</v>
       </c>
-      <c r="P17" s="1">
-        <v>1000</v>
-      </c>
-      <c r="Q17" s="1" t="s">
+      <c r="P17" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q17" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="R17" s="1" t="s">
+      <c r="R17" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="S17" s="1">
+      <c r="S17" s="3">
         <v>500</v>
       </c>
-      <c r="T17" s="1">
+      <c r="T17" s="3">
         <v>10</v>
       </c>
-      <c r="U17" s="1" t="s">
+      <c r="U17" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="V17" s="1" t="s">
+      <c r="V17" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="W17" s="1">
+      <c r="W17" s="3">
         <v>8500</v>
       </c>
-      <c r="X17" s="1" t="s">
+      <c r="X17" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:24" ht="58" x14ac:dyDescent="0.35">
-      <c r="B18" s="1">
+      <c r="B18" s="3">
         <v>2</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="4">
         <v>42872</v>
       </c>
-      <c r="D18" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0</v>
-      </c>
-      <c r="F18" s="1">
-        <v>0</v>
-      </c>
-      <c r="G18" s="1" t="s">
+      <c r="D18" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18" s="3">
         <v>100</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="J18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K18" s="1">
-        <v>10000</v>
-      </c>
-      <c r="L18" s="1">
-        <v>10000</v>
-      </c>
-      <c r="M18" s="1" t="s">
+      <c r="K18" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L18" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M18" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N18" s="1">
+      <c r="N18" s="3">
         <v>1E-3</v>
       </c>
-      <c r="O18" s="1">
+      <c r="O18" s="3">
         <v>0.9</v>
       </c>
-      <c r="P18" s="1">
-        <v>1000</v>
-      </c>
-      <c r="Q18" s="1" t="s">
+      <c r="P18" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q18" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="R18" s="1" t="s">
+      <c r="R18" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="S18" s="1">
+      <c r="S18" s="3">
         <v>500</v>
       </c>
-      <c r="T18" s="1">
+      <c r="T18" s="3">
         <v>10</v>
       </c>
-      <c r="U18" s="1" t="s">
+      <c r="U18" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="V18" s="1" t="s">
+      <c r="V18" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="W18" s="1">
+      <c r="W18" s="3">
         <v>8600</v>
       </c>
     </row>
     <row r="19" spans="1:24" ht="58" x14ac:dyDescent="0.35">
-      <c r="B19" s="1">
+      <c r="B19" s="3">
         <v>1</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="4">
         <v>42872</v>
       </c>
-      <c r="D19" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-      <c r="F19" s="1">
-        <v>0</v>
-      </c>
-      <c r="G19" s="1" t="s">
+      <c r="D19" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I19" s="3">
         <v>100</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="J19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K19" s="1">
-        <v>10000</v>
-      </c>
-      <c r="L19" s="1">
-        <v>10000</v>
-      </c>
-      <c r="M19" s="1" t="s">
+      <c r="K19" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L19" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M19" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N19" s="1">
+      <c r="N19" s="3">
         <v>1E-3</v>
       </c>
-      <c r="O19" s="1">
+      <c r="O19" s="3">
         <v>0.9</v>
       </c>
-      <c r="P19" s="1">
-        <v>1000</v>
-      </c>
-      <c r="Q19" s="1" t="s">
+      <c r="P19" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q19" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="R19" s="1" t="s">
+      <c r="R19" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="S19" s="1">
+      <c r="S19" s="3">
         <v>500</v>
       </c>
-      <c r="T19" s="1">
+      <c r="T19" s="3">
         <v>10</v>
       </c>
-      <c r="U19" s="1" t="s">
+      <c r="U19" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="V19" s="1" t="s">
+      <c r="V19" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="W19" s="1">
+      <c r="W19" s="3">
         <v>2200</v>
       </c>
     </row>
     <row r="20" spans="1:24" ht="58" x14ac:dyDescent="0.35">
-      <c r="B20" s="1">
+      <c r="B20" s="3">
         <v>1</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="4">
         <v>42872</v>
       </c>
-      <c r="D20" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0</v>
-      </c>
-      <c r="F20" s="1">
-        <v>0</v>
-      </c>
-      <c r="G20" s="1" t="s">
+      <c r="D20" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20" s="3">
         <v>100</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="K20" s="1">
-        <v>10000</v>
-      </c>
-      <c r="L20" s="1">
-        <v>10000</v>
-      </c>
-      <c r="M20" s="1" t="s">
+      <c r="K20" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L20" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N20" s="1">
+      <c r="N20" s="3">
         <v>1E-3</v>
       </c>
-      <c r="O20" s="1">
+      <c r="O20" s="3">
         <v>0.9</v>
       </c>
-      <c r="P20" s="1">
-        <v>1000</v>
-      </c>
-      <c r="Q20" s="1" t="s">
+      <c r="P20" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q20" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="R20" s="1" t="s">
+      <c r="R20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="S20" s="1">
+      <c r="S20" s="3">
         <v>500</v>
       </c>
-      <c r="T20" s="1">
+      <c r="T20" s="3">
         <v>10</v>
       </c>
-      <c r="U20" s="1" t="s">
+      <c r="U20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="V20" s="1" t="s">
+      <c r="V20" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="W20" s="1">
+      <c r="W20" s="3">
         <v>4100</v>
       </c>
-      <c r="X20" s="1" t="s">
+      <c r="X20" s="3" t="s">
         <v>67</v>
       </c>
+    </row>
+    <row r="21" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1</v>
+      </c>
+      <c r="C21" s="4">
+        <v>42875</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21" s="3">
+        <v>100</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K21" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L21" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N21" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="O21" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="P21" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="R21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S21" s="3">
+        <v>5000</v>
+      </c>
+      <c r="T21" s="3">
+        <v>10</v>
+      </c>
+      <c r="U21" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="V21" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W21" s="3">
+        <v>67700</v>
+      </c>
+      <c r="X21" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+      <c r="C22" s="4">
+        <v>42875</v>
+      </c>
+      <c r="D22" s="3">
+        <v>8000</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="3">
+        <v>100</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L22" s="3">
+        <v>10000</v>
+      </c>
+      <c r="M22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N22" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="O22" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="P22" s="3">
+        <v>1000</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="R22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S22" s="3">
+        <v>5000</v>
+      </c>
+      <c r="T22" s="3">
+        <v>10</v>
+      </c>
+      <c r="U22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="V22" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="W22" s="3">
+        <v>19900</v>
+      </c>
+      <c r="X22" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="C23" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added to thesis document, added stochascity to DRQN, added softmax to DDQN
</commit_message>
<xml_diff>
--- a/Proposed Architecture/results.xlsx
+++ b/Proposed Architecture/results.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="77">
   <si>
     <t>DAL</t>
   </si>
@@ -246,6 +246,15 @@
   </si>
   <si>
     <t>8 episodes, 4 length</t>
+  </si>
+  <si>
+    <t>8 episodes, 32 length, epsilon of 0.9, decay of 0.1 every 5000 epochs, with reward of 20, -20 and penalty of -1, scheduled shared replay of 1, 0.125, 10000</t>
+  </si>
+  <si>
+    <t>28\125</t>
+  </si>
+  <si>
+    <t>8 episodes, 32 length, epsilon of 0.9, decay of 0.1 every 10000 epochs, with reward of 100, -100 and penalty of -1, scheduled shared replay of 1, 0.125, 10000</t>
   </si>
 </sst>
 </file>
@@ -295,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment textRotation="255" wrapText="1"/>
@@ -310,6 +319,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -626,11 +638,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y23"/>
+  <dimension ref="A1:Y25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W26" sqref="W26"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W32" sqref="W32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -645,15 +657,18 @@
     <col min="8" max="8" width="9.6328125" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.08984375" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="6.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6" style="3" customWidth="1"/>
+    <col min="12" max="12" width="7.54296875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="6.08984375" style="3" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="3.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="6.08984375" style="3" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6.1796875" style="3" customWidth="1"/>
     <col min="18" max="18" width="7.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.7265625" style="3"/>
+    <col min="20" max="23" width="8.7265625" style="3"/>
+    <col min="24" max="24" width="39.81640625" style="3" customWidth="1"/>
+    <col min="25" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="2" customFormat="1" ht="137.5" x14ac:dyDescent="0.35">
@@ -2217,8 +2232,218 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="C23" s="4"/>
+    <row r="23" spans="1:24" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="B23" s="3">
+        <v>2</v>
+      </c>
+      <c r="C23" s="4">
+        <v>42880</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I23" s="3">
+        <v>100</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K23" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L23" s="3">
+        <v>100000</v>
+      </c>
+      <c r="M23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N23" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="O23" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="P23" s="3">
+        <v>20</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>1</v>
+      </c>
+      <c r="R23" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S23" s="3">
+        <v>500</v>
+      </c>
+      <c r="T23" s="3">
+        <v>10</v>
+      </c>
+      <c r="U23" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="V23" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="W23" s="3">
+        <v>55200</v>
+      </c>
+      <c r="X23" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" ht="304.5" x14ac:dyDescent="0.35">
+      <c r="B24" s="3">
+        <v>3</v>
+      </c>
+      <c r="C24" s="4">
+        <v>42880</v>
+      </c>
+      <c r="D24" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" s="3">
+        <v>100</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K24" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L24" s="3">
+        <v>100000</v>
+      </c>
+      <c r="M24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N24" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="O24" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="P24" s="3">
+        <v>100</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>1</v>
+      </c>
+      <c r="R24" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S24" s="3">
+        <v>500</v>
+      </c>
+      <c r="T24" s="3">
+        <v>10</v>
+      </c>
+      <c r="U24" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="V24" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="W24" s="3">
+        <v>99100</v>
+      </c>
+      <c r="X24" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" ht="58" x14ac:dyDescent="0.35">
+      <c r="B25" s="3">
+        <v>4</v>
+      </c>
+      <c r="C25" s="4">
+        <v>42880</v>
+      </c>
+      <c r="D25" s="3">
+        <v>1000</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I25" s="3">
+        <v>100</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K25" s="3">
+        <v>10000</v>
+      </c>
+      <c r="L25" s="3">
+        <v>100000</v>
+      </c>
+      <c r="M25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N25" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="O25" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="P25" s="3">
+        <v>100</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="R25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="S25" s="3">
+        <v>500</v>
+      </c>
+      <c r="T25" s="3">
+        <v>10</v>
+      </c>
+      <c r="U25" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="V25" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="W25" s="3">
+        <v>88000</v>
+      </c>
+      <c r="X25" s="6" t="s">
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>